<commit_message>
Changes in results structure
</commit_message>
<xml_diff>
--- a/data_and_results/yearly data/2099.xlsx
+++ b/data_and_results/yearly data/2099.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20736" windowHeight="11760" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20736" windowHeight="11760" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="01" sheetId="2" r:id="rId1"/>
@@ -10616,8 +10616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA140"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14150,7 +14150,7 @@
   <dimension ref="A1:AA140"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17687,7 +17687,7 @@
   <dimension ref="A1:AA140"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18060,7 +18060,7 @@
         <v>0</v>
       </c>
       <c r="M9" s="16">
-        <f t="shared" si="1"/>
+        <f>SUM(M11:M706)</f>
         <v>0</v>
       </c>
       <c r="N9" s="16">
@@ -18072,15 +18072,15 @@
         <v>0</v>
       </c>
       <c r="P9" s="16">
-        <f t="shared" si="1"/>
+        <f>SUM(P11:P706)</f>
         <v>0</v>
       </c>
       <c r="Q9" s="16">
-        <f t="shared" si="1"/>
+        <f>SUM(Q11:Q706)</f>
         <v>0</v>
       </c>
       <c r="R9" s="16">
-        <f t="shared" si="1"/>
+        <f>SUM(R11:R706)</f>
         <v>0</v>
       </c>
       <c r="S9" s="17">
@@ -35408,7 +35408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA140"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
@@ -42464,7 +42464,7 @@
   <dimension ref="A1:AA140"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+      <selection activeCell="Q10" sqref="Q10:Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -42791,11 +42791,11 @@
         <v>707.3</v>
       </c>
       <c r="C9" s="16">
-        <f t="shared" ref="C9:T9" si="1">SUM(C11:C706)</f>
+        <f>SUM(C11:C706)</f>
         <v>900</v>
       </c>
       <c r="D9" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="D9:T9" si="1">SUM(D11:D706)</f>
         <v>12</v>
       </c>
       <c r="E9" s="16">
@@ -42847,7 +42847,7 @@
         <v>0</v>
       </c>
       <c r="Q9" s="16">
-        <f t="shared" si="1"/>
+        <f>SUM(Q11:Q706)</f>
         <v>0</v>
       </c>
       <c r="R9" s="16">

</xml_diff>